<commit_message>
Imputed HK rain data using Quarry Bay and Cape rainfall station
</commit_message>
<xml_diff>
--- a/dat/climate/HKCM.xlsx
+++ b/dat/climate/HKCM.xlsx
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6817" uniqueCount="873">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6732" uniqueCount="871">
   <si>
     <t>year</t>
   </si>
@@ -2649,12 +2649,6 @@
   <si>
     <t>   4.4#</t>
   </si>
-  <si>
-    <t>0#</t>
-  </si>
-  <si>
-    <t>85#</t>
-  </si>
 </sst>
 </file>
 
@@ -3079,8 +3073,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M201"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
-      <selection activeCell="G118" sqref="G118"/>
+    <sheetView tabSelected="1" topLeftCell="A180" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2:K201"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3160,8 +3154,8 @@
       <c r="J2" s="3">
         <v>74</v>
       </c>
-      <c r="K2" s="3" t="s">
-        <v>431</v>
+      <c r="K2" s="3">
+        <v>22.75</v>
       </c>
       <c r="L2" s="3" t="s">
         <v>79</v>
@@ -3201,8 +3195,8 @@
       <c r="J3" s="5">
         <v>75</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>431</v>
+      <c r="K3" s="5">
+        <v>4.5</v>
       </c>
       <c r="L3" s="5">
         <v>100</v>
@@ -3242,8 +3236,8 @@
       <c r="J4" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="K4" s="3" t="s">
-        <v>431</v>
+      <c r="K4" s="3">
+        <v>198.75</v>
       </c>
       <c r="L4" s="3">
         <v>110</v>
@@ -3283,8 +3277,8 @@
       <c r="J5" s="5">
         <v>81</v>
       </c>
-      <c r="K5" s="5" t="s">
-        <v>431</v>
+      <c r="K5" s="5">
+        <v>19</v>
       </c>
       <c r="L5" s="5">
         <v>120</v>
@@ -3324,8 +3318,8 @@
       <c r="J6" s="3">
         <v>81</v>
       </c>
-      <c r="K6" s="3" t="s">
-        <v>431</v>
+      <c r="K6" s="3">
+        <v>299.5</v>
       </c>
       <c r="L6" s="3">
         <v>120</v>
@@ -3365,8 +3359,8 @@
       <c r="J7" s="5">
         <v>82</v>
       </c>
-      <c r="K7" s="5" t="s">
-        <v>431</v>
+      <c r="K7" s="5">
+        <v>174</v>
       </c>
       <c r="L7" s="5">
         <v>120</v>
@@ -3406,8 +3400,8 @@
       <c r="J8" s="3">
         <v>84</v>
       </c>
-      <c r="K8" s="3" t="s">
-        <v>431</v>
+      <c r="K8" s="3">
+        <v>265.5</v>
       </c>
       <c r="L8" s="3">
         <v>130</v>
@@ -3447,8 +3441,8 @@
       <c r="J9" s="3">
         <v>82</v>
       </c>
-      <c r="K9" s="3" t="s">
-        <v>431</v>
+      <c r="K9" s="3">
+        <v>308.5</v>
       </c>
       <c r="L9" s="3">
         <v>110</v>
@@ -3488,8 +3482,8 @@
       <c r="J10" s="5">
         <v>78</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>431</v>
+      <c r="K10" s="5">
+        <v>592.25</v>
       </c>
       <c r="L10" s="5">
         <v>110</v>
@@ -3529,8 +3523,8 @@
       <c r="J11" s="3">
         <v>76</v>
       </c>
-      <c r="K11" s="3" t="s">
-        <v>431</v>
+      <c r="K11" s="3">
+        <v>156</v>
       </c>
       <c r="L11" s="3">
         <v>100</v>
@@ -3570,8 +3564,8 @@
       <c r="J12" s="5">
         <v>71</v>
       </c>
-      <c r="K12" s="5" t="s">
-        <v>431</v>
+      <c r="K12" s="5">
+        <v>18</v>
       </c>
       <c r="L12" s="5">
         <v>100</v>
@@ -3611,8 +3605,8 @@
       <c r="J13" s="3">
         <v>77</v>
       </c>
-      <c r="K13" s="3" t="s">
-        <v>431</v>
+      <c r="K13" s="3">
+        <v>54</v>
       </c>
       <c r="L13" s="3">
         <v>100</v>
@@ -3652,8 +3646,8 @@
       <c r="J14" s="5">
         <v>70</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>431</v>
+      <c r="K14" s="5">
+        <v>20.25</v>
       </c>
       <c r="L14" s="5">
         <v>100</v>
@@ -3693,8 +3687,8 @@
       <c r="J15" s="3">
         <v>80</v>
       </c>
-      <c r="K15" s="3" t="s">
-        <v>431</v>
+      <c r="K15" s="3">
+        <v>14.75</v>
       </c>
       <c r="L15" s="3">
         <v>110</v>
@@ -3734,8 +3728,8 @@
       <c r="J16" s="3">
         <v>79</v>
       </c>
-      <c r="K16" s="3" t="s">
-        <v>431</v>
+      <c r="K16" s="3">
+        <v>59.75</v>
       </c>
       <c r="L16" s="3">
         <v>100</v>
@@ -3775,8 +3769,8 @@
       <c r="J17" s="5">
         <v>82</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>431</v>
+      <c r="K17" s="5">
+        <v>85</v>
       </c>
       <c r="L17" s="5">
         <v>110</v>
@@ -3816,8 +3810,8 @@
       <c r="J18" s="3">
         <v>82</v>
       </c>
-      <c r="K18" s="3" t="s">
-        <v>431</v>
+      <c r="K18" s="3">
+        <v>337</v>
       </c>
       <c r="L18" s="3">
         <v>120</v>
@@ -3857,8 +3851,8 @@
       <c r="J19" s="5">
         <v>86</v>
       </c>
-      <c r="K19" s="5" t="s">
-        <v>431</v>
+      <c r="K19" s="5">
+        <v>458</v>
       </c>
       <c r="L19" s="5">
         <v>130</v>
@@ -3898,8 +3892,8 @@
       <c r="J20" s="3" t="s">
         <v>337</v>
       </c>
-      <c r="K20" s="3" t="s">
-        <v>431</v>
+      <c r="K20" s="3">
+        <v>73.75</v>
       </c>
       <c r="L20" s="3">
         <v>120</v>
@@ -3939,8 +3933,8 @@
       <c r="J21" s="5">
         <v>84</v>
       </c>
-      <c r="K21" s="5" t="s">
-        <v>431</v>
+      <c r="K21" s="5">
+        <v>342.75</v>
       </c>
       <c r="L21" s="5">
         <v>120</v>
@@ -3980,8 +3974,8 @@
       <c r="J22" s="3">
         <v>82</v>
       </c>
-      <c r="K22" s="3" t="s">
-        <v>431</v>
+      <c r="K22" s="3">
+        <v>363.25</v>
       </c>
       <c r="L22" s="3">
         <v>110</v>
@@ -4021,8 +4015,8 @@
       <c r="J23" s="3">
         <v>73</v>
       </c>
-      <c r="K23" s="3" t="s">
-        <v>431</v>
+      <c r="K23" s="3">
+        <v>31</v>
       </c>
       <c r="L23" s="3">
         <v>110</v>
@@ -4062,8 +4056,8 @@
       <c r="J24" s="5">
         <v>74</v>
       </c>
-      <c r="K24" s="5" t="s">
-        <v>431</v>
+      <c r="K24" s="5">
+        <v>82.75</v>
       </c>
       <c r="L24" s="5">
         <v>100</v>
@@ -4103,8 +4097,8 @@
       <c r="J25" s="3">
         <v>66</v>
       </c>
-      <c r="K25" s="3" t="s">
-        <v>431</v>
+      <c r="K25" s="3">
+        <v>0</v>
       </c>
       <c r="L25" s="3">
         <v>100</v>
@@ -4144,8 +4138,8 @@
       <c r="J26" s="5">
         <v>72</v>
       </c>
-      <c r="K26" s="5" t="s">
-        <v>431</v>
+      <c r="K26" s="5">
+        <v>36.5</v>
       </c>
       <c r="L26" s="5">
         <v>100</v>
@@ -4185,8 +4179,8 @@
       <c r="J27" s="3">
         <v>79</v>
       </c>
-      <c r="K27" s="3" t="s">
-        <v>431</v>
+      <c r="K27" s="3">
+        <v>45.5</v>
       </c>
       <c r="L27" s="3">
         <v>100</v>
@@ -4226,8 +4220,8 @@
       <c r="J28" s="5">
         <v>81</v>
       </c>
-      <c r="K28" s="5" t="s">
-        <v>431</v>
+      <c r="K28" s="5">
+        <v>91.75</v>
       </c>
       <c r="L28" s="5">
         <v>110</v>
@@ -4267,8 +4261,8 @@
       <c r="J29" s="3">
         <v>84</v>
       </c>
-      <c r="K29" s="3" t="s">
-        <v>431</v>
+      <c r="K29" s="3">
+        <v>159.75</v>
       </c>
       <c r="L29" s="3">
         <v>120</v>
@@ -4308,8 +4302,8 @@
       <c r="J30" s="3">
         <v>83</v>
       </c>
-      <c r="K30" s="3" t="s">
-        <v>431</v>
+      <c r="K30" s="3">
+        <v>138.5</v>
       </c>
       <c r="L30" s="3">
         <v>130</v>
@@ -4349,8 +4343,8 @@
       <c r="J31" s="5">
         <v>80</v>
       </c>
-      <c r="K31" s="5" t="s">
-        <v>431</v>
+      <c r="K31" s="5">
+        <v>109.25</v>
       </c>
       <c r="L31" s="5">
         <v>120</v>
@@ -4390,8 +4384,8 @@
       <c r="J32" s="3">
         <v>84</v>
       </c>
-      <c r="K32" s="3" t="s">
-        <v>431</v>
+      <c r="K32" s="3">
+        <v>326</v>
       </c>
       <c r="L32" s="3">
         <v>110</v>
@@ -4431,8 +4425,8 @@
       <c r="J33" s="5">
         <v>85</v>
       </c>
-      <c r="K33" s="5" t="s">
-        <v>431</v>
+      <c r="K33" s="5">
+        <v>387.25</v>
       </c>
       <c r="L33" s="5">
         <v>130</v>
@@ -4472,8 +4466,8 @@
       <c r="J34" s="3">
         <v>80</v>
       </c>
-      <c r="K34" s="3" t="s">
-        <v>431</v>
+      <c r="K34" s="3">
+        <v>165.75</v>
       </c>
       <c r="L34" s="3">
         <v>120</v>
@@ -4513,8 +4507,8 @@
       <c r="J35" s="5">
         <v>66</v>
       </c>
-      <c r="K35" s="5" t="s">
-        <v>431</v>
+      <c r="K35" s="5">
+        <v>8.25</v>
       </c>
       <c r="L35" s="5">
         <v>110</v>
@@ -4554,8 +4548,8 @@
       <c r="J36" s="3">
         <v>71</v>
       </c>
-      <c r="K36" s="3" t="s">
-        <v>431</v>
+      <c r="K36" s="3">
+        <v>0.5</v>
       </c>
       <c r="L36" s="3">
         <v>110</v>
@@ -4595,8 +4589,8 @@
       <c r="J37" s="3">
         <v>68</v>
       </c>
-      <c r="K37" s="3" t="s">
-        <v>431</v>
+      <c r="K37" s="3">
+        <v>0</v>
       </c>
       <c r="L37" s="3">
         <v>100</v>
@@ -4636,8 +4630,8 @@
       <c r="J38" s="5">
         <v>75</v>
       </c>
-      <c r="K38" s="5" t="s">
-        <v>431</v>
+      <c r="K38" s="5">
+        <v>4</v>
       </c>
       <c r="L38" s="5">
         <v>100</v>
@@ -4677,8 +4671,8 @@
       <c r="J39" s="3">
         <v>84</v>
       </c>
-      <c r="K39" s="3" t="s">
-        <v>431</v>
+      <c r="K39" s="3">
+        <v>24</v>
       </c>
       <c r="L39" s="3">
         <v>110</v>
@@ -4718,8 +4712,8 @@
       <c r="J40" s="5">
         <v>76</v>
       </c>
-      <c r="K40" s="5" t="s">
-        <v>431</v>
+      <c r="K40" s="5">
+        <v>47.25</v>
       </c>
       <c r="L40" s="5">
         <v>110</v>
@@ -4759,8 +4753,8 @@
       <c r="J41" s="3">
         <v>83</v>
       </c>
-      <c r="K41" s="3" t="s">
-        <v>431</v>
+      <c r="K41" s="3">
+        <v>36</v>
       </c>
       <c r="L41" s="3">
         <v>130</v>
@@ -4800,8 +4794,8 @@
       <c r="J42" s="5">
         <v>87</v>
       </c>
-      <c r="K42" s="5" t="s">
-        <v>431</v>
+      <c r="K42" s="5">
+        <v>555.75</v>
       </c>
       <c r="L42" s="5">
         <v>120</v>
@@ -4841,8 +4835,8 @@
       <c r="J43" s="3">
         <v>88</v>
       </c>
-      <c r="K43" s="3" t="s">
-        <v>431</v>
+      <c r="K43" s="3">
+        <v>696</v>
       </c>
       <c r="L43" s="3">
         <v>110</v>
@@ -4882,8 +4876,8 @@
       <c r="J44" s="3">
         <v>83</v>
       </c>
-      <c r="K44" s="3" t="s">
-        <v>431</v>
+      <c r="K44" s="3">
+        <v>287</v>
       </c>
       <c r="L44" s="3" t="s">
         <v>431</v>
@@ -4923,8 +4917,8 @@
       <c r="J45" s="5">
         <v>87</v>
       </c>
-      <c r="K45" s="5" t="s">
-        <v>431</v>
+      <c r="K45" s="5">
+        <v>767</v>
       </c>
       <c r="L45" s="5" t="s">
         <v>431</v>
@@ -4964,8 +4958,8 @@
       <c r="J46" s="3">
         <v>80</v>
       </c>
-      <c r="K46" s="3" t="s">
-        <v>431</v>
+      <c r="K46" s="3">
+        <v>284</v>
       </c>
       <c r="L46" s="3" t="s">
         <v>123</v>
@@ -5005,8 +4999,8 @@
       <c r="J47" s="5">
         <v>71</v>
       </c>
-      <c r="K47" s="5" t="s">
-        <v>431</v>
+      <c r="K47" s="5">
+        <v>15.75</v>
       </c>
       <c r="L47" s="5" t="s">
         <v>79</v>
@@ -5046,8 +5040,8 @@
       <c r="J48" s="3">
         <v>72</v>
       </c>
-      <c r="K48" s="3" t="s">
-        <v>431</v>
+      <c r="K48" s="3">
+        <v>0.75</v>
       </c>
       <c r="L48" s="3">
         <v>100</v>
@@ -5087,8 +5081,8 @@
       <c r="J49" s="5">
         <v>56</v>
       </c>
-      <c r="K49" s="5" t="s">
-        <v>431</v>
+      <c r="K49" s="5">
+        <v>9</v>
       </c>
       <c r="L49" s="5">
         <v>100</v>
@@ -5128,8 +5122,8 @@
       <c r="J50" s="3">
         <v>72</v>
       </c>
-      <c r="K50" s="3" t="s">
-        <v>431</v>
+      <c r="K50" s="3">
+        <v>16.25</v>
       </c>
       <c r="L50" s="3">
         <v>100</v>
@@ -5169,8 +5163,8 @@
       <c r="J51" s="3">
         <v>75</v>
       </c>
-      <c r="K51" s="3" t="s">
-        <v>431</v>
+      <c r="K51" s="3">
+        <v>37.5</v>
       </c>
       <c r="L51" s="3">
         <v>110</v>
@@ -5210,8 +5204,8 @@
       <c r="J52" s="5">
         <v>78</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>431</v>
+      <c r="K52" s="5">
+        <v>52.5</v>
       </c>
       <c r="L52" s="5">
         <v>100</v>
@@ -5251,8 +5245,8 @@
       <c r="J53" s="3">
         <v>82</v>
       </c>
-      <c r="K53" s="3" t="s">
-        <v>431</v>
+      <c r="K53" s="3">
+        <v>129.75</v>
       </c>
       <c r="L53" s="3">
         <v>120</v>
@@ -5292,8 +5286,8 @@
       <c r="J54" s="5">
         <v>83</v>
       </c>
-      <c r="K54" s="5" t="s">
-        <v>431</v>
+      <c r="K54" s="5">
+        <v>335.25</v>
       </c>
       <c r="L54" s="5">
         <v>120</v>
@@ -5333,8 +5327,8 @@
       <c r="J55" s="3">
         <v>86</v>
       </c>
-      <c r="K55" s="3" t="s">
-        <v>431</v>
+      <c r="K55" s="3">
+        <v>281.75</v>
       </c>
       <c r="L55" s="3">
         <v>120</v>
@@ -5374,8 +5368,8 @@
       <c r="J56" s="5">
         <v>82</v>
       </c>
-      <c r="K56" s="5" t="s">
-        <v>431</v>
+      <c r="K56" s="5">
+        <v>481.75</v>
       </c>
       <c r="L56" s="5">
         <v>120</v>
@@ -5415,8 +5409,8 @@
       <c r="J57" s="3">
         <v>81</v>
       </c>
-      <c r="K57" s="3" t="s">
-        <v>431</v>
+      <c r="K57" s="3">
+        <v>178</v>
       </c>
       <c r="L57" s="3">
         <v>120</v>
@@ -5456,8 +5450,8 @@
       <c r="J58" s="3">
         <v>76</v>
       </c>
-      <c r="K58" s="3" t="s">
-        <v>431</v>
+      <c r="K58" s="3">
+        <v>382.5</v>
       </c>
       <c r="L58" s="3">
         <v>110</v>
@@ -5497,8 +5491,8 @@
       <c r="J59" s="5">
         <v>73</v>
       </c>
-      <c r="K59" s="5" t="s">
-        <v>431</v>
+      <c r="K59" s="5">
+        <v>7</v>
       </c>
       <c r="L59" s="5">
         <v>110</v>
@@ -5538,8 +5532,8 @@
       <c r="J60" s="3">
         <v>73</v>
       </c>
-      <c r="K60" s="3" t="s">
-        <v>431</v>
+      <c r="K60" s="3">
+        <v>84</v>
       </c>
       <c r="L60" s="3">
         <v>100</v>
@@ -5579,8 +5573,8 @@
       <c r="J61" s="5">
         <v>65</v>
       </c>
-      <c r="K61" s="5" t="s">
-        <v>431</v>
+      <c r="K61" s="5">
+        <v>25.5</v>
       </c>
       <c r="L61" s="5">
         <v>100</v>
@@ -5620,8 +5614,8 @@
       <c r="J62" s="3">
         <v>66</v>
       </c>
-      <c r="K62" s="3" t="s">
-        <v>431</v>
+      <c r="K62" s="3">
+        <v>31.75</v>
       </c>
       <c r="L62" s="3">
         <v>100</v>
@@ -5661,8 +5655,8 @@
       <c r="J63" s="5">
         <v>74</v>
       </c>
-      <c r="K63" s="5" t="s">
-        <v>431</v>
+      <c r="K63" s="5">
+        <v>13.75</v>
       </c>
       <c r="L63" s="5">
         <v>110</v>
@@ -5702,8 +5696,8 @@
       <c r="J64" s="3">
         <v>81</v>
       </c>
-      <c r="K64" s="3" t="s">
-        <v>431</v>
+      <c r="K64" s="3">
+        <v>24</v>
       </c>
       <c r="L64" s="3">
         <v>110</v>
@@ -5743,8 +5737,8 @@
       <c r="J65" s="3">
         <v>79</v>
       </c>
-      <c r="K65" s="3" t="s">
-        <v>431</v>
+      <c r="K65" s="3">
+        <v>134.25</v>
       </c>
       <c r="L65" s="3">
         <v>120</v>
@@ -5784,8 +5778,8 @@
       <c r="J66" s="5">
         <v>81</v>
       </c>
-      <c r="K66" s="5" t="s">
-        <v>431</v>
+      <c r="K66" s="5">
+        <v>329.5</v>
       </c>
       <c r="L66" s="5">
         <v>120</v>
@@ -5825,8 +5819,8 @@
       <c r="J67" s="3">
         <v>85</v>
       </c>
-      <c r="K67" s="3" t="s">
-        <v>431</v>
+      <c r="K67" s="3">
+        <v>491</v>
       </c>
       <c r="L67" s="3">
         <v>140</v>
@@ -5866,8 +5860,8 @@
       <c r="J68" s="5">
         <v>81</v>
       </c>
-      <c r="K68" s="5" t="s">
-        <v>431</v>
+      <c r="K68" s="5">
+        <v>69</v>
       </c>
       <c r="L68" s="5">
         <v>130</v>
@@ -5907,8 +5901,8 @@
       <c r="J69" s="3">
         <v>84</v>
       </c>
-      <c r="K69" s="3" t="s">
-        <v>431</v>
+      <c r="K69" s="3">
+        <v>422</v>
       </c>
       <c r="L69" s="3">
         <v>120</v>
@@ -5948,8 +5942,8 @@
       <c r="J70" s="5">
         <v>74</v>
       </c>
-      <c r="K70" s="5" t="s">
-        <v>431</v>
+      <c r="K70" s="5">
+        <v>112.75</v>
       </c>
       <c r="L70" s="5">
         <v>110</v>
@@ -5989,8 +5983,8 @@
       <c r="J71" s="3">
         <v>70</v>
       </c>
-      <c r="K71" s="3" t="s">
-        <v>431</v>
+      <c r="K71" s="3">
+        <v>45.75</v>
       </c>
       <c r="L71" s="3">
         <v>100</v>
@@ -6030,8 +6024,8 @@
       <c r="J72" s="3">
         <v>61</v>
       </c>
-      <c r="K72" s="3" t="s">
-        <v>431</v>
+      <c r="K72" s="3">
+        <v>2.5</v>
       </c>
       <c r="L72" s="3">
         <v>100</v>
@@ -6071,8 +6065,8 @@
       <c r="J73" s="5">
         <v>70</v>
       </c>
-      <c r="K73" s="5" t="s">
-        <v>431</v>
+      <c r="K73" s="5">
+        <v>19</v>
       </c>
       <c r="L73" s="5">
         <v>100</v>
@@ -6112,8 +6106,8 @@
       <c r="J74" s="3">
         <v>71</v>
       </c>
-      <c r="K74" s="3" t="s">
-        <v>431</v>
+      <c r="K74" s="3">
+        <v>24.25</v>
       </c>
       <c r="L74" s="3">
         <v>100</v>
@@ -6153,8 +6147,8 @@
       <c r="J75" s="5">
         <v>66</v>
       </c>
-      <c r="K75" s="5" t="s">
-        <v>431</v>
+      <c r="K75" s="5">
+        <v>22.75</v>
       </c>
       <c r="L75" s="5">
         <v>110</v>
@@ -6194,8 +6188,8 @@
       <c r="J76" s="3">
         <v>72</v>
       </c>
-      <c r="K76" s="3" t="s">
-        <v>431</v>
+      <c r="K76" s="3">
+        <v>76.25</v>
       </c>
       <c r="L76" s="3">
         <v>110</v>
@@ -6235,8 +6229,8 @@
       <c r="J77" s="5">
         <v>82</v>
       </c>
-      <c r="K77" s="5" t="s">
-        <v>431</v>
+      <c r="K77" s="5">
+        <v>183.75</v>
       </c>
       <c r="L77" s="5">
         <v>120</v>
@@ -6276,8 +6270,8 @@
       <c r="J78" s="3">
         <v>81</v>
       </c>
-      <c r="K78" s="3" t="s">
-        <v>431</v>
+      <c r="K78" s="3">
+        <v>143.75</v>
       </c>
       <c r="L78" s="3">
         <v>110</v>
@@ -6317,8 +6311,8 @@
       <c r="J79" s="3">
         <v>89</v>
       </c>
-      <c r="K79" s="3" t="s">
-        <v>431</v>
+      <c r="K79" s="3">
+        <v>1174</v>
       </c>
       <c r="L79" s="3">
         <v>130</v>
@@ -6358,8 +6352,8 @@
       <c r="J80" s="5">
         <v>85</v>
       </c>
-      <c r="K80" s="5" t="s">
-        <v>431</v>
+      <c r="K80" s="5">
+        <v>450.75</v>
       </c>
       <c r="L80" s="5">
         <v>140</v>
@@ -6399,8 +6393,8 @@
       <c r="J81" s="3">
         <v>82</v>
       </c>
-      <c r="K81" s="3" t="s">
-        <v>431</v>
+      <c r="K81" s="3">
+        <v>251.25</v>
       </c>
       <c r="L81" s="3">
         <v>130</v>
@@ -6440,8 +6434,8 @@
       <c r="J82" s="5">
         <v>76</v>
       </c>
-      <c r="K82" s="5" t="s">
-        <v>431</v>
+      <c r="K82" s="5">
+        <v>111.25</v>
       </c>
       <c r="L82" s="5">
         <v>110</v>
@@ -6481,8 +6475,8 @@
       <c r="J83" s="3">
         <v>75</v>
       </c>
-      <c r="K83" s="3" t="s">
-        <v>431</v>
+      <c r="K83" s="3">
+        <v>88.75</v>
       </c>
       <c r="L83" s="3">
         <v>110</v>
@@ -6522,8 +6516,8 @@
       <c r="J84" s="5" t="s">
         <v>853</v>
       </c>
-      <c r="K84" s="5" t="s">
-        <v>431</v>
+      <c r="K84" s="5">
+        <v>8.75</v>
       </c>
       <c r="L84" s="5">
         <v>100</v>
@@ -6564,7 +6558,7 @@
         <v>60</v>
       </c>
       <c r="K85" s="3">
-        <v>9.5</v>
+        <v>9.375</v>
       </c>
       <c r="L85" s="3">
         <v>120</v>
@@ -6646,7 +6640,7 @@
         <v>309</v>
       </c>
       <c r="K87" s="5">
-        <v>5.5</v>
+        <v>4.5</v>
       </c>
       <c r="L87" s="5">
         <v>130</v>
@@ -6687,7 +6681,7 @@
         <v>81</v>
       </c>
       <c r="K88" s="3">
-        <v>133.5</v>
+        <v>130.875</v>
       </c>
       <c r="L88" s="3">
         <v>110</v>
@@ -6728,7 +6722,7 @@
         <v>76</v>
       </c>
       <c r="K89" s="5">
-        <v>94.5</v>
+        <v>103.25</v>
       </c>
       <c r="L89" s="5">
         <v>110</v>
@@ -6769,7 +6763,7 @@
         <v>78</v>
       </c>
       <c r="K90" s="3">
-        <v>188</v>
+        <v>187.75</v>
       </c>
       <c r="L90" s="3">
         <v>110</v>
@@ -6810,7 +6804,7 @@
         <v>86</v>
       </c>
       <c r="K91" s="5">
-        <v>324</v>
+        <v>350.75</v>
       </c>
       <c r="L91" s="5">
         <v>130</v>
@@ -6851,7 +6845,7 @@
         <v>83</v>
       </c>
       <c r="K92" s="3">
-        <v>423</v>
+        <v>384.75</v>
       </c>
       <c r="L92" s="3">
         <v>110</v>
@@ -6892,7 +6886,7 @@
         <v>83</v>
       </c>
       <c r="K93" s="3">
-        <v>351</v>
+        <v>287.375</v>
       </c>
       <c r="L93" s="3">
         <v>140</v>
@@ -6933,7 +6927,7 @@
         <v>77</v>
       </c>
       <c r="K94" s="5">
-        <v>628.5</v>
+        <v>539.625</v>
       </c>
       <c r="L94" s="5">
         <v>100</v>
@@ -6974,7 +6968,7 @@
         <v>73</v>
       </c>
       <c r="K95" s="3">
-        <v>34.5</v>
+        <v>23.375</v>
       </c>
       <c r="L95" s="3">
         <v>100</v>
@@ -7015,7 +7009,7 @@
         <v>69</v>
       </c>
       <c r="K96" s="5">
-        <v>40</v>
+        <v>56.5</v>
       </c>
       <c r="L96" s="5">
         <v>90</v>
@@ -7056,7 +7050,7 @@
         <v>74</v>
       </c>
       <c r="K97" s="3">
-        <v>36</v>
+        <v>41</v>
       </c>
       <c r="L97" s="3">
         <v>90</v>
@@ -7097,7 +7091,7 @@
         <v>74</v>
       </c>
       <c r="K98" s="5">
-        <v>25.5</v>
+        <v>24.625</v>
       </c>
       <c r="L98" s="5">
         <v>90</v>
@@ -7138,7 +7132,7 @@
         <v>85</v>
       </c>
       <c r="K99" s="3">
-        <v>81.5</v>
+        <v>85.5</v>
       </c>
       <c r="L99" s="3">
         <v>90</v>
@@ -7178,8 +7172,8 @@
       <c r="J100" s="3">
         <v>75</v>
       </c>
-      <c r="K100" s="3" t="s">
-        <v>871</v>
+      <c r="K100" s="3">
+        <v>5.25</v>
       </c>
       <c r="L100" s="3">
         <v>100</v>
@@ -7219,8 +7213,8 @@
       <c r="J101" s="5">
         <v>82</v>
       </c>
-      <c r="K101" s="5" t="s">
-        <v>872</v>
+      <c r="K101" s="5">
+        <v>91.75</v>
       </c>
       <c r="L101" s="5">
         <v>90</v>
@@ -7261,7 +7255,7 @@
         <v>84</v>
       </c>
       <c r="K102" s="3">
-        <v>199.5</v>
+        <v>185.625</v>
       </c>
       <c r="L102" s="3">
         <v>100</v>
@@ -7302,7 +7296,7 @@
         <v>88</v>
       </c>
       <c r="K103" s="5">
-        <v>418</v>
+        <v>446.5</v>
       </c>
       <c r="L103" s="5">
         <v>140</v>
@@ -7343,7 +7337,7 @@
         <v>84</v>
       </c>
       <c r="K104" s="3">
-        <v>434.5</v>
+        <v>406.5</v>
       </c>
       <c r="L104" s="3">
         <v>250</v>
@@ -7384,7 +7378,7 @@
         <v>82</v>
       </c>
       <c r="K105" s="5">
-        <v>279.5</v>
+        <v>251</v>
       </c>
       <c r="L105" s="5">
         <v>100</v>
@@ -7425,7 +7419,7 @@
         <v>83</v>
       </c>
       <c r="K106" s="3">
-        <v>658.5</v>
+        <v>643.875</v>
       </c>
       <c r="L106" s="3" t="s">
         <v>79</v>
@@ -7466,7 +7460,7 @@
         <v>67</v>
       </c>
       <c r="K107" s="7">
-        <v>20.5</v>
+        <v>33.25</v>
       </c>
       <c r="L107" s="7">
         <v>90</v>
@@ -7507,7 +7501,7 @@
         <v>71</v>
       </c>
       <c r="K108" s="9">
-        <v>37</v>
+        <v>35.75</v>
       </c>
       <c r="L108" s="9">
         <v>90</v>
@@ -7548,7 +7542,7 @@
         <v>64</v>
       </c>
       <c r="K109" s="7">
-        <v>21.5</v>
+        <v>18.25</v>
       </c>
       <c r="L109" s="7">
         <v>90</v>
@@ -7589,7 +7583,7 @@
         <v>63</v>
       </c>
       <c r="K110" s="3">
-        <v>5</v>
+        <v>4.125</v>
       </c>
       <c r="L110" s="3">
         <v>80</v>
@@ -7630,7 +7624,7 @@
         <v>75</v>
       </c>
       <c r="K111" s="5">
-        <v>22.5</v>
+        <v>21.375</v>
       </c>
       <c r="L111" s="5">
         <v>80</v>
@@ -7671,7 +7665,7 @@
         <v>68</v>
       </c>
       <c r="K112" s="3">
-        <v>23.5</v>
+        <v>22.375</v>
       </c>
       <c r="L112" s="3">
         <v>80</v>
@@ -7712,7 +7706,7 @@
         <v>77</v>
       </c>
       <c r="K113" s="5">
-        <v>33.5</v>
+        <v>37.875</v>
       </c>
       <c r="L113" s="5">
         <v>90</v>
@@ -7753,7 +7747,7 @@
         <v>82</v>
       </c>
       <c r="K114" s="3">
-        <v>166</v>
+        <v>169.75</v>
       </c>
       <c r="L114" s="3">
         <v>130</v>
@@ -7794,7 +7788,7 @@
         <v>85</v>
       </c>
       <c r="K115" s="5">
-        <v>412.5</v>
+        <v>407</v>
       </c>
       <c r="L115" s="5">
         <v>130</v>
@@ -7835,7 +7829,7 @@
         <v>156</v>
       </c>
       <c r="K116" s="3">
-        <v>198.5</v>
+        <v>214.875</v>
       </c>
       <c r="L116" s="3">
         <v>240</v>
@@ -7876,7 +7870,7 @@
         <v>80</v>
       </c>
       <c r="K117" s="5">
-        <v>184</v>
+        <v>146.5</v>
       </c>
       <c r="L117" s="5">
         <v>230</v>
@@ -7917,7 +7911,7 @@
         <v>265</v>
       </c>
       <c r="K118" s="3">
-        <v>150</v>
+        <v>140.75</v>
       </c>
       <c r="L118" s="3" t="s">
         <v>158</v>
@@ -7958,7 +7952,7 @@
         <v>74</v>
       </c>
       <c r="K119" s="5">
-        <v>151.5</v>
+        <v>141.25</v>
       </c>
       <c r="L119" s="5">
         <v>90</v>
@@ -7999,7 +7993,7 @@
         <v>487</v>
       </c>
       <c r="K120" s="3">
-        <v>94</v>
+        <v>94.25</v>
       </c>
       <c r="L120" s="3" t="s">
         <v>158</v>
@@ -8040,7 +8034,7 @@
         <v>568</v>
       </c>
       <c r="K121" s="5">
-        <v>3.5</v>
+        <v>2.75</v>
       </c>
       <c r="L121" s="5" t="s">
         <v>294</v>
@@ -8081,7 +8075,7 @@
         <v>77</v>
       </c>
       <c r="K122" s="3">
-        <v>37</v>
+        <v>36.75</v>
       </c>
       <c r="L122" s="3">
         <v>80</v>
@@ -8122,7 +8116,7 @@
         <v>77</v>
       </c>
       <c r="K123" s="5">
-        <v>27</v>
+        <v>30.625</v>
       </c>
       <c r="L123" s="5">
         <v>80</v>
@@ -8163,7 +8157,7 @@
         <v>76</v>
       </c>
       <c r="K124" s="3">
-        <v>20.5</v>
+        <v>15.625</v>
       </c>
       <c r="L124" s="3">
         <v>90</v>
@@ -8204,7 +8198,7 @@
         <v>84</v>
       </c>
       <c r="K125" s="5">
-        <v>269</v>
+        <v>285.625</v>
       </c>
       <c r="L125" s="5">
         <v>90</v>
@@ -8245,7 +8239,7 @@
         <v>84</v>
       </c>
       <c r="K126" s="3">
-        <v>342</v>
+        <v>333.25</v>
       </c>
       <c r="L126" s="3">
         <v>90</v>
@@ -8286,7 +8280,7 @@
         <v>82</v>
       </c>
       <c r="K127" s="5">
-        <v>243</v>
+        <v>224.375</v>
       </c>
       <c r="L127" s="5">
         <v>100</v>
@@ -8327,7 +8321,7 @@
         <v>82</v>
       </c>
       <c r="K128" s="3">
-        <v>411.5</v>
+        <v>375</v>
       </c>
       <c r="L128" s="3">
         <v>130</v>
@@ -8368,7 +8362,7 @@
         <v>79</v>
       </c>
       <c r="K129" s="5">
-        <v>178.5</v>
+        <v>167.75</v>
       </c>
       <c r="L129" s="5">
         <v>230</v>
@@ -8409,7 +8403,7 @@
         <v>74</v>
       </c>
       <c r="K130" s="3">
-        <v>214.5</v>
+        <v>195</v>
       </c>
       <c r="L130" s="3">
         <v>90</v>
@@ -8450,7 +8444,7 @@
         <v>71</v>
       </c>
       <c r="K131" s="5">
-        <v>51</v>
+        <v>43.75</v>
       </c>
       <c r="L131" s="5">
         <v>90</v>
@@ -8491,7 +8485,7 @@
         <v>77</v>
       </c>
       <c r="K132" s="3">
-        <v>42</v>
+        <v>51.75</v>
       </c>
       <c r="L132" s="3">
         <v>90</v>
@@ -8532,7 +8526,7 @@
         <v>72</v>
       </c>
       <c r="K133" s="5">
-        <v>51</v>
+        <v>47.25</v>
       </c>
       <c r="L133" s="5">
         <v>90</v>
@@ -8573,7 +8567,7 @@
         <v>67</v>
       </c>
       <c r="K134" s="3">
-        <v>3</v>
+        <v>3.25</v>
       </c>
       <c r="L134" s="3">
         <v>80</v>
@@ -8614,7 +8608,7 @@
         <v>77</v>
       </c>
       <c r="K135" s="5">
-        <v>1</v>
+        <v>2.25</v>
       </c>
       <c r="L135" s="5">
         <v>90</v>
@@ -8655,7 +8649,7 @@
         <v>77</v>
       </c>
       <c r="K136" s="3">
-        <v>151</v>
+        <v>130.875</v>
       </c>
       <c r="L136" s="3">
         <v>90</v>
@@ -8696,7 +8690,7 @@
         <v>82</v>
       </c>
       <c r="K137" s="5">
-        <v>172.5</v>
+        <v>169.125</v>
       </c>
       <c r="L137" s="5">
         <v>90</v>
@@ -8737,7 +8731,7 @@
         <v>87</v>
       </c>
       <c r="K138" s="3">
-        <v>417</v>
+        <v>391.25</v>
       </c>
       <c r="L138" s="3">
         <v>130</v>
@@ -8778,7 +8772,7 @@
         <v>84</v>
       </c>
       <c r="K139" s="5">
-        <v>375</v>
+        <v>343.875</v>
       </c>
       <c r="L139" s="5">
         <v>100</v>
@@ -8819,7 +8813,7 @@
         <v>84</v>
       </c>
       <c r="K140" s="3">
-        <v>477</v>
+        <v>426.375</v>
       </c>
       <c r="L140" s="3">
         <v>90</v>
@@ -8860,7 +8854,7 @@
         <v>83</v>
       </c>
       <c r="K141" s="5">
-        <v>404</v>
+        <v>341.5</v>
       </c>
       <c r="L141" s="5">
         <v>90</v>
@@ -8901,7 +8895,7 @@
         <v>77</v>
       </c>
       <c r="K142" s="3">
-        <v>374</v>
+        <v>341.5</v>
       </c>
       <c r="L142" s="3">
         <v>90</v>
@@ -8942,7 +8936,7 @@
         <v>65</v>
       </c>
       <c r="K143" s="5">
-        <v>1</v>
+        <v>1.375</v>
       </c>
       <c r="L143" s="5">
         <v>90</v>
@@ -8983,7 +8977,7 @@
         <v>65</v>
       </c>
       <c r="K144" s="3">
-        <v>64.5</v>
+        <v>59.625</v>
       </c>
       <c r="L144" s="3">
         <v>90</v>
@@ -9024,7 +9018,7 @@
         <v>55</v>
       </c>
       <c r="K145" s="5">
-        <v>79</v>
+        <v>73.875</v>
       </c>
       <c r="L145" s="5">
         <v>80</v>
@@ -9065,7 +9059,7 @@
         <v>60</v>
       </c>
       <c r="K146" s="3">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="L146" s="3">
         <v>80</v>
@@ -9106,7 +9100,7 @@
         <v>74</v>
       </c>
       <c r="K147" s="5">
-        <v>37</v>
+        <v>35.25</v>
       </c>
       <c r="L147" s="5">
         <v>80</v>
@@ -9147,7 +9141,7 @@
         <v>77</v>
       </c>
       <c r="K148" s="3">
-        <v>159</v>
+        <v>155.625</v>
       </c>
       <c r="L148" s="3">
         <v>80</v>
@@ -9188,7 +9182,7 @@
         <v>81</v>
       </c>
       <c r="K149" s="5">
-        <v>109.5</v>
+        <v>121.25</v>
       </c>
       <c r="L149" s="5">
         <v>90</v>
@@ -9229,7 +9223,7 @@
         <v>87</v>
       </c>
       <c r="K150" s="3">
-        <v>781</v>
+        <v>738.625</v>
       </c>
       <c r="L150" s="3">
         <v>90</v>
@@ -9270,7 +9264,7 @@
         <v>82</v>
       </c>
       <c r="K151" s="5">
-        <v>409.5</v>
+        <v>402.5</v>
       </c>
       <c r="L151" s="5">
         <v>120</v>
@@ -9311,7 +9305,7 @@
         <v>81</v>
       </c>
       <c r="K152" s="3">
-        <v>233.5</v>
+        <v>225.5</v>
       </c>
       <c r="L152" s="3">
         <v>240</v>
@@ -9352,7 +9346,7 @@
         <v>83</v>
       </c>
       <c r="K153" s="5">
-        <v>487.5</v>
+        <v>511.625</v>
       </c>
       <c r="L153" s="5">
         <v>230</v>
@@ -9393,7 +9387,7 @@
         <v>79</v>
       </c>
       <c r="K154" s="3">
-        <v>173</v>
+        <v>134.875</v>
       </c>
       <c r="L154" s="3">
         <v>130</v>
@@ -9434,7 +9428,7 @@
         <v>69</v>
       </c>
       <c r="K155" s="5">
-        <v>79</v>
+        <v>109.875</v>
       </c>
       <c r="L155" s="5">
         <v>100</v>
@@ -9475,7 +9469,7 @@
         <v>74</v>
       </c>
       <c r="K156" s="3">
-        <v>47.5</v>
+        <v>54.5</v>
       </c>
       <c r="L156" s="3">
         <v>90</v>
@@ -9516,7 +9510,7 @@
         <v>61</v>
       </c>
       <c r="K157" s="5">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="L157" s="5">
         <v>90</v>
@@ -9557,7 +9551,7 @@
         <v>67</v>
       </c>
       <c r="K158" s="3">
-        <v>39</v>
+        <v>37.125</v>
       </c>
       <c r="L158" s="3">
         <v>80</v>
@@ -9598,7 +9592,7 @@
         <v>73</v>
       </c>
       <c r="K159" s="5">
-        <v>25</v>
+        <v>25.625</v>
       </c>
       <c r="L159" s="5">
         <v>80</v>
@@ -9639,7 +9633,7 @@
         <v>80</v>
       </c>
       <c r="K160" s="3">
-        <v>18.5</v>
+        <v>19.5</v>
       </c>
       <c r="L160" s="3">
         <v>130</v>
@@ -9680,7 +9674,7 @@
         <v>77</v>
       </c>
       <c r="K161" s="5">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="L161" s="5">
         <v>130</v>
@@ -9721,7 +9715,7 @@
         <v>88</v>
       </c>
       <c r="K162" s="3">
-        <v>457.5</v>
+        <v>476.375</v>
       </c>
       <c r="L162" s="3">
         <v>120</v>
@@ -9762,7 +9756,7 @@
         <v>83</v>
       </c>
       <c r="K163" s="5">
-        <v>304.5</v>
+        <v>195</v>
       </c>
       <c r="L163" s="5">
         <v>230</v>
@@ -9803,7 +9797,7 @@
         <v>82</v>
       </c>
       <c r="K164" s="3">
-        <v>477</v>
+        <v>436.875</v>
       </c>
       <c r="L164" s="3">
         <v>130</v>
@@ -9844,7 +9838,7 @@
         <v>27</v>
       </c>
       <c r="K165" s="5">
-        <v>153.5</v>
+        <v>172.375</v>
       </c>
       <c r="L165" s="5">
         <v>130</v>
@@ -9885,7 +9879,7 @@
         <v>270</v>
       </c>
       <c r="K166" s="3">
-        <v>103.5</v>
+        <v>114</v>
       </c>
       <c r="L166" s="3">
         <v>90</v>
@@ -9926,7 +9920,7 @@
         <v>76</v>
       </c>
       <c r="K167" s="5">
-        <v>149.5</v>
+        <v>126.5</v>
       </c>
       <c r="L167" s="5">
         <v>90</v>
@@ -9967,7 +9961,7 @@
         <v>75</v>
       </c>
       <c r="K168" s="3">
-        <v>16</v>
+        <v>22.75</v>
       </c>
       <c r="L168" s="3">
         <v>90</v>
@@ -10008,7 +10002,7 @@
         <v>72</v>
       </c>
       <c r="K169" s="5">
-        <v>66</v>
+        <v>63.375</v>
       </c>
       <c r="L169" s="5">
         <v>80</v>
@@ -10049,7 +10043,7 @@
         <v>77</v>
       </c>
       <c r="K170" s="3">
-        <v>197</v>
+        <v>207.25</v>
       </c>
       <c r="L170" s="3">
         <v>80</v>
@@ -10090,7 +10084,7 @@
         <v>68</v>
       </c>
       <c r="K171" s="5">
-        <v>22</v>
+        <v>23.5</v>
       </c>
       <c r="L171" s="5">
         <v>80</v>
@@ -10131,7 +10125,7 @@
         <v>79</v>
       </c>
       <c r="K172" s="3">
-        <v>166.5</v>
+        <v>168</v>
       </c>
       <c r="L172" s="3">
         <v>80</v>
@@ -10172,7 +10166,7 @@
         <v>88</v>
       </c>
       <c r="K173" s="5">
-        <v>239.5</v>
+        <v>228</v>
       </c>
       <c r="L173" s="5">
         <v>130</v>
@@ -10213,7 +10207,7 @@
         <v>84</v>
       </c>
       <c r="K174" s="3">
-        <v>173.5</v>
+        <v>180.25</v>
       </c>
       <c r="L174" s="3">
         <v>90</v>
@@ -10254,7 +10248,7 @@
         <v>85</v>
       </c>
       <c r="K175" s="5">
-        <v>390.5</v>
+        <v>356.125</v>
       </c>
       <c r="L175" s="5">
         <v>130</v>
@@ -10295,7 +10289,7 @@
         <v>81</v>
       </c>
       <c r="K176" s="3">
-        <v>194</v>
+        <v>202.125</v>
       </c>
       <c r="L176" s="3">
         <v>230</v>
@@ -10336,7 +10330,7 @@
         <v>84</v>
       </c>
       <c r="K177" s="5">
-        <v>465</v>
+        <v>457.25</v>
       </c>
       <c r="L177" s="5">
         <v>120</v>
@@ -10377,7 +10371,7 @@
         <v>245</v>
       </c>
       <c r="K178" s="3">
-        <v>294</v>
+        <v>311.75</v>
       </c>
       <c r="L178" s="3" t="s">
         <v>294</v>
@@ -10418,7 +10412,7 @@
         <v>292</v>
       </c>
       <c r="K179" s="5">
-        <v>591.5</v>
+        <v>533.125</v>
       </c>
       <c r="L179" s="5" t="s">
         <v>862</v>
@@ -10459,7 +10453,7 @@
         <v>76</v>
       </c>
       <c r="K180" s="3">
-        <v>136.5</v>
+        <v>131.5</v>
       </c>
       <c r="L180" s="3">
         <v>70</v>
@@ -10500,7 +10494,7 @@
         <v>66</v>
       </c>
       <c r="K181" s="5">
-        <v>8.5</v>
+        <v>9.5</v>
       </c>
       <c r="L181" s="5">
         <v>70</v>
@@ -10541,7 +10535,7 @@
         <v>292</v>
       </c>
       <c r="K182" s="3">
-        <v>14</v>
+        <v>9.625</v>
       </c>
       <c r="L182" s="3">
         <v>70</v>
@@ -10582,7 +10576,7 @@
         <v>69</v>
       </c>
       <c r="K183" s="5">
-        <v>15.5</v>
+        <v>17.625</v>
       </c>
       <c r="L183" s="5">
         <v>70</v>
@@ -10623,7 +10617,7 @@
         <v>75</v>
       </c>
       <c r="K184" s="3">
-        <v>40</v>
+        <v>40.625</v>
       </c>
       <c r="L184" s="3">
         <v>70</v>
@@ -10664,7 +10658,7 @@
         <v>81</v>
       </c>
       <c r="K185" s="5">
-        <v>72.5</v>
+        <v>74</v>
       </c>
       <c r="L185" s="5">
         <v>70</v>
@@ -10705,7 +10699,7 @@
         <v>86</v>
       </c>
       <c r="K186" s="3">
-        <v>299</v>
+        <v>280.125</v>
       </c>
       <c r="L186" s="3">
         <v>120</v>
@@ -10746,7 +10740,7 @@
         <v>121</v>
       </c>
       <c r="K187" s="5">
-        <v>646.5</v>
+        <v>635</v>
       </c>
       <c r="L187" s="5" t="s">
         <v>99</v>
@@ -10787,7 +10781,7 @@
         <v>90</v>
       </c>
       <c r="K188" s="3">
-        <v>623</v>
+        <v>606.625</v>
       </c>
       <c r="L188" s="3" t="s">
         <v>512</v>
@@ -10828,7 +10822,7 @@
         <v>80</v>
       </c>
       <c r="K189" s="5">
-        <v>502.5</v>
+        <v>466.125</v>
       </c>
       <c r="L189" s="5">
         <v>220</v>
@@ -10869,7 +10863,7 @@
         <v>79</v>
       </c>
       <c r="K190" s="3">
-        <v>241</v>
+        <v>214.875</v>
       </c>
       <c r="L190" s="3">
         <v>80</v>
@@ -10910,7 +10904,7 @@
         <v>64</v>
       </c>
       <c r="K191" s="5">
-        <v>91.5</v>
+        <v>83.875</v>
       </c>
       <c r="L191" s="5">
         <v>80</v>
@@ -10951,7 +10945,7 @@
         <v>163</v>
       </c>
       <c r="K192" s="3">
-        <v>33</v>
+        <v>30.875</v>
       </c>
       <c r="L192" s="3">
         <v>70</v>
@@ -10992,7 +10986,7 @@
         <v>57</v>
       </c>
       <c r="K193" s="5">
-        <v>0</v>
+        <v>0.125</v>
       </c>
       <c r="L193" s="5">
         <v>60</v>
@@ -11033,7 +11027,7 @@
         <v>70</v>
       </c>
       <c r="K194" s="3">
-        <v>64.5</v>
+        <v>59.875</v>
       </c>
       <c r="L194" s="3">
         <v>70</v>
@@ -11074,7 +11068,7 @@
         <v>67</v>
       </c>
       <c r="K195" s="5">
-        <v>7.5</v>
+        <v>6.625</v>
       </c>
       <c r="L195" s="5">
         <v>110</v>
@@ -11115,7 +11109,7 @@
         <v>73</v>
       </c>
       <c r="K196" s="3">
-        <v>25</v>
+        <v>24.5</v>
       </c>
       <c r="L196" s="3">
         <v>70</v>
@@ -11156,7 +11150,7 @@
         <v>76</v>
       </c>
       <c r="K197" s="5">
-        <v>44.5</v>
+        <v>37.5</v>
       </c>
       <c r="L197" s="5">
         <v>120</v>
@@ -11197,7 +11191,7 @@
         <v>79</v>
       </c>
       <c r="K198" s="3">
-        <v>70</v>
+        <v>73.625</v>
       </c>
       <c r="L198" s="3">
         <v>220</v>
@@ -11238,7 +11232,7 @@
         <v>81</v>
       </c>
       <c r="K199" s="5">
-        <v>480.5</v>
+        <v>501.125</v>
       </c>
       <c r="L199" s="5" t="s">
         <v>294</v>
@@ -11279,7 +11273,7 @@
         <v>85</v>
       </c>
       <c r="K200" s="3">
-        <v>355</v>
+        <v>326.875</v>
       </c>
       <c r="L200" s="3" t="s">
         <v>123</v>
@@ -11320,7 +11314,7 @@
         <v>88</v>
       </c>
       <c r="K201" s="5">
-        <v>717</v>
+        <v>592.25</v>
       </c>
       <c r="L201" s="5">
         <v>50</v>

</xml_diff>